<commit_message>
tracking sheets by city
</commit_message>
<xml_diff>
--- a/data/Confirmation/clean/confirmation_summary.xlsx
+++ b/data/Confirmation/clean/confirmation_summary.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t xml:space="preserve">provincia</t>
   </si>
@@ -116,9 +116,6 @@
     <t xml:space="preserve">Namaacha</t>
   </si>
   <si>
-    <t xml:space="preserve">Ponta De Ouro</t>
-  </si>
-  <si>
     <t xml:space="preserve">Nampula</t>
   </si>
   <si>
@@ -134,10 +131,16 @@
     <t xml:space="preserve">Beira</t>
   </si>
   <si>
+    <t xml:space="preserve">Buzi</t>
+  </si>
+  <si>
     <t xml:space="preserve">Caia</t>
   </si>
   <si>
     <t xml:space="preserve">Dondo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Muchungue</t>
   </si>
   <si>
     <t xml:space="preserve">Nhamantada</t>
@@ -736,7 +739,7 @@
         <v>25</v>
       </c>
       <c r="C18" t="n">
-        <v>829</v>
+        <v>817</v>
       </c>
       <c r="D18" t="s">
         <v>6</v>
@@ -750,7 +753,7 @@
         <v>27</v>
       </c>
       <c r="C19" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D19" t="s">
         <v>6</v>
@@ -778,7 +781,7 @@
         <v>29</v>
       </c>
       <c r="C21" t="n">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="D21" t="s">
         <v>6</v>
@@ -820,7 +823,7 @@
         <v>32</v>
       </c>
       <c r="C24" t="n">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D24" t="s">
         <v>6</v>
@@ -834,7 +837,7 @@
         <v>33</v>
       </c>
       <c r="C25" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D25" t="s">
         <v>6</v>
@@ -842,10 +845,10 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="B26" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C26" t="n">
         <v>1</v>
@@ -856,7 +859,7 @@
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B27" t="s">
         <v>36</v>
@@ -870,13 +873,13 @@
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B28" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C28" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D28" t="s">
         <v>6</v>
@@ -884,13 +887,13 @@
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B29" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C29" t="n">
-        <v>4</v>
+        <v>164</v>
       </c>
       <c r="D29" t="s">
         <v>6</v>
@@ -898,13 +901,13 @@
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B30" t="s">
         <v>39</v>
       </c>
       <c r="C30" t="n">
-        <v>168</v>
+        <v>1</v>
       </c>
       <c r="D30" t="s">
         <v>6</v>
@@ -912,7 +915,7 @@
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B31" t="s">
         <v>40</v>
@@ -926,7 +929,7 @@
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B32" t="s">
         <v>41</v>
@@ -940,7 +943,7 @@
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B33" t="s">
         <v>42</v>
@@ -954,13 +957,13 @@
     </row>
     <row r="34">
       <c r="A34" t="s">
+        <v>37</v>
+      </c>
+      <c r="B34" t="s">
         <v>43</v>
       </c>
-      <c r="B34" t="s">
-        <v>44</v>
-      </c>
       <c r="C34" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D34" t="s">
         <v>6</v>
@@ -968,13 +971,13 @@
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B35" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C35" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D35" t="s">
         <v>6</v>
@@ -982,13 +985,13 @@
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B36" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C36" t="n">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="D36" t="s">
         <v>6</v>
@@ -996,13 +999,13 @@
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B37" t="s">
         <v>47</v>
       </c>
       <c r="C37" t="n">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="D37" t="s">
         <v>6</v>
@@ -1010,15 +1013,29 @@
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B38" t="s">
         <v>48</v>
       </c>
       <c r="C38" t="n">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="D38" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s">
+        <v>46</v>
+      </c>
+      <c r="B39" t="s">
+        <v>49</v>
+      </c>
+      <c r="C39" t="n">
+        <v>1</v>
+      </c>
+      <c r="D39" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>